<commit_message>
finished double pendulum lab
</commit_message>
<xml_diff>
--- a/IB/labs/double_pendulum/exercises1234.xlsx
+++ b/IB/labs/double_pendulum/exercises1234.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\MEng-CW\IB\labs\double_pendulum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39E7CB13-7109-4961-AE8B-9C91F688588C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D40C2E6-06C3-46E0-ABB5-22D2F2388F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exercises1234" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>1. Experiment</t>
   </si>
@@ -56,11 +56,23 @@
   <si>
     <t>5. Experiment</t>
   </si>
+  <si>
+    <t>MODE 1</t>
+  </si>
+  <si>
+    <t>MODE 2</t>
+  </si>
+  <si>
+    <t>MIXED MODE</t>
+  </si>
+  <si>
+    <t>HIGH ANGLE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37629,7 +37641,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
@@ -37640,7 +37652,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
@@ -37651,7 +37663,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
@@ -37662,7 +37674,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
@@ -37673,7 +37685,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
@@ -38144,11 +38156,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:TU34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38157,6 +38169,9 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:541" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -43053,6 +43068,9 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:541" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -47949,6 +47967,9 @@
       <c r="A15" t="s">
         <v>7</v>
       </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:541" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -52845,6 +52866,9 @@
       <c r="A22" t="s">
         <v>8</v>
       </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23" spans="1:541" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -57734,6 +57758,9 @@
     <row r="29" spans="1:541" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:541" x14ac:dyDescent="0.25">

</xml_diff>